<commit_message>
add PI Loop Filter
</commit_message>
<xml_diff>
--- a/300_iir_llpf_calc.xlsx
+++ b/300_iir_llpf_calc.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204A4F9A-0A14-454E-B4CB-88D56DD671A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13785" yWindow="1080" windowWidth="13800" windowHeight="15675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoopFilter LPF" sheetId="4" r:id="rId1"/>
@@ -12,9 +18,9 @@
     <sheet name="2nd order LPFz" sheetId="1" r:id="rId3"/>
     <sheet name="LFz" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -146,8 +152,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -255,7 +261,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -307,7 +313,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -501,34 +507,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -539,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -550,7 +556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -562,7 +568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -577,7 +583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -592,7 +598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -604,7 +610,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -613,7 +619,7 @@
         <v>2.0218174810193945</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -622,7 +628,7 @@
         <v>1.9781825189806053</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -634,7 +640,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -646,7 +652,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -658,7 +664,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -666,7 +672,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -675,7 +681,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -687,7 +693,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -699,7 +705,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -720,38 +726,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>175</v>
+        <v>600</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -762,19 +768,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <f>2*PI()*B2</f>
-        <v>1099.5574287564275</v>
+        <v>3769.9111843077517</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -789,13 +795,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>1099.691011647627</v>
+        <v>3775.3034581577217</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -804,73 +810,73 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
         <f>B6*B5</f>
-        <v>3.8183715682209268E-2</v>
+        <v>0.13108692563047644</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
         <f>2+(B8)</f>
-        <v>2.0381837156822091</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>2.1310869256304765</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
         <f>2-B8</f>
-        <v>1.9618162843177906</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>1.8689130743695235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <f>B10/B9</f>
-        <v>0.96253162520295321</v>
+        <v>0.87697646299275678</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13">
         <f>B8/B9</f>
-        <v>1.8734187398523412E-2</v>
+        <v>6.1511768503621556E-2</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <f>B8/B9</f>
-        <v>1.8734187398523412E-2</v>
+        <v>6.1511768503621556E-2</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -878,7 +884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -887,37 +893,37 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18">
         <f>ROUND(B17*B13,0)</f>
-        <v>614</v>
+        <v>2016</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19">
         <f>ROUND(B17*B14,0)</f>
-        <v>614</v>
+        <v>2016</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20">
         <f>ROUND(B17*B12,0)</f>
-        <v>31540</v>
+        <v>28737</v>
       </c>
       <c r="D20" t="s">
         <v>20</v>
@@ -932,27 +938,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -963,7 +969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -974,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -986,7 +992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1016,7 +1022,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1028,7 +1034,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1037,7 +1043,7 @@
         <v>2.3078294421196581</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1046,7 +1052,7 @@
         <v>1.6921705578803419</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.25">
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.25">
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>0.64930619341182005</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1089,7 +1095,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>1.9083729945233441E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1106,7 +1112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1115,7 +1121,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1127,7 +1133,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1139,7 +1145,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1148,7 +1154,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1160,7 +1166,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1178,39 +1184,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>480</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1221,19 +1227,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <f>2*PI()*B2</f>
-        <v>3015.9289474462012</v>
+        <v>628.31853071795865</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1248,13 +1254,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>3018.6880867031732</v>
+        <v>628.34345335856813</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1263,43 +1269,43 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
         <f>B6*B5</f>
-        <v>0.10481555856608241</v>
+        <v>2.1817481019394725E-2</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
         <f>2+(B8)</f>
-        <v>2.1048155585660826</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>2.0218174810193945</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
       <c r="B10">
         <f>B8-2</f>
-        <v>-1.8951844414339176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>-1.9781825189806053</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
       <c r="B11">
         <f>1/(2*B6)</f>
-        <v>1.6563486708097406E-4</v>
+        <v>7.9574315181839229E-4</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
@@ -1308,16 +1314,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12">
         <f>B11*1000000</f>
-        <v>165.63486708097406</v>
+        <v>795.74315181839233</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1328,90 +1334,90 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15">
         <f>B9</f>
-        <v>2.1048155585660826</v>
+        <v>2.0218174810193945</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16">
         <f>B10</f>
-        <v>-1.8951844414339176</v>
+        <v>-1.9781825189806053</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
       <c r="B19">
         <f>POWER(2,B18)</f>
-        <v>32768</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20">
         <f>ROUND(B19*B15,0)</f>
-        <v>68971</v>
+        <v>16563</v>
       </c>
       <c r="D20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21">
         <f>ROUND(B16*B19,0)</f>
-        <v>-62101</v>
+        <v>-16205</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22">
         <f>ROUND(B19*B14,0)</f>
-        <v>32768</v>
+        <v>8192</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
       <c r="B23">
         <f>1/(B11*B6*2)</f>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
costas work 300 bpsk h
</commit_message>
<xml_diff>
--- a/300_iir_llpf_calc.xlsx
+++ b/300_iir_llpf_calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204A4F9A-0A14-454E-B4CB-88D56DD671A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD65618A-B2EB-0247-A585-887C0E6594D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoopFilter LPF" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="37">
   <si>
     <t>cutoff freq</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>a2 scaled</t>
+  </si>
+  <si>
+    <t>Gain</t>
   </si>
 </sst>
 </file>
@@ -515,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,54 +669,62 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16">
         <v>8</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <f>POWER(2,B16)</f>
-        <v>32768</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B18">
-        <f>ROUND(B17*B13,0)</f>
-        <v>354</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B19">
-        <f>ROUND(B17*B14,0)</f>
-        <v>354</v>
-      </c>
-      <c r="D19" t="s">
-        <v>21</v>
+        <f>POWER(2,B18)</f>
+        <v>32768</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <f>ROUND(B19*B13*B16,0)</f>
+        <v>2829</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <f>ROUND(B19*B14*B16,0)</f>
+        <v>2829</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B20">
-        <f>ROUND(B17*B12,0)</f>
+      <c r="B22">
+        <f>ROUND(B19*B12,0)</f>
         <v>32061</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -727,10 +738,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,54 +889,62 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <f>POWER(2,B16)</f>
-        <v>32768</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B18">
-        <f>ROUND(B17*B13,0)</f>
-        <v>2016</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B19">
-        <f>ROUND(B17*B14,0)</f>
-        <v>2016</v>
-      </c>
-      <c r="D19" t="s">
-        <v>21</v>
+        <f>POWER(2,B18)</f>
+        <v>32768</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <f>ROUND(B19*B13*B16,0)</f>
+        <v>8062</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <f>ROUND(B19*B14*B16,0)</f>
+        <v>8062</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B20">
-        <f>ROUND(B17*B12,0)</f>
+      <c r="B22">
+        <f>ROUND(B19*B12,0)</f>
         <v>28737</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1187,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1384,7 +1403,7 @@
         <v>16563</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1408,7 +1427,7 @@
         <v>8192</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Costas 2nd order loop filter
</commit_message>
<xml_diff>
--- a/300_iir_llpf_calc.xlsx
+++ b/300_iir_llpf_calc.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD65618A-B2EB-0247-A585-887C0E6594D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955878D5-8D44-DA4F-9EC7-84057CF228E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoopFilter LPF" sheetId="4" r:id="rId1"/>
-    <sheet name="Branch LPF" sheetId="3" r:id="rId2"/>
-    <sheet name="2nd order LPFz" sheetId="1" r:id="rId3"/>
-    <sheet name="LFz" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Branch LPF" sheetId="3" r:id="rId3"/>
+    <sheet name="2nd order LPFz" sheetId="1" r:id="rId4"/>
+    <sheet name="LFz" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="49">
   <si>
     <t>cutoff freq</t>
   </si>
@@ -150,6 +151,42 @@
   </si>
   <si>
     <t>Gain</t>
+  </si>
+  <si>
+    <t>B0=b0^2</t>
+  </si>
+  <si>
+    <t>B1=2b0b1</t>
+  </si>
+  <si>
+    <t>B2=b1^2</t>
+  </si>
+  <si>
+    <t>First Order system</t>
+  </si>
+  <si>
+    <t>Second Order system</t>
+  </si>
+  <si>
+    <t>A1=2a1</t>
+  </si>
+  <si>
+    <t>A2=-a1^2</t>
+  </si>
+  <si>
+    <t>B0_scaled</t>
+  </si>
+  <si>
+    <t>B1_scaled</t>
+  </si>
+  <si>
+    <t>B2_scaled</t>
+  </si>
+  <si>
+    <t>A1_scaled</t>
+  </si>
+  <si>
+    <t>A2_scaled</t>
   </si>
 </sst>
 </file>
@@ -198,10 +235,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -520,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -672,7 +712,7 @@
         <v>36</v>
       </c>
       <c r="B16">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -698,7 +738,7 @@
       </c>
       <c r="B20">
         <f>ROUND(B19*B13*B16,0)</f>
-        <v>2829</v>
+        <v>354</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
@@ -710,7 +750,7 @@
       </c>
       <c r="B21">
         <f>ROUND(B19*B14*B16,0)</f>
-        <v>2829</v>
+        <v>354</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -737,11 +777,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0218B47B-13FF-3F43-B902-FE92EE5440FF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -887,76 +939,235 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B18">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19">
-        <f>POWER(2,B18)</f>
-        <v>32768</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B20">
-        <f>ROUND(B19*B13*B16,0)</f>
-        <v>8062</v>
-      </c>
-      <c r="D20" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B21">
-        <f>ROUND(B19*B14*B16,0)</f>
-        <v>8062</v>
-      </c>
-      <c r="D21" t="s">
-        <v>21</v>
+        <f>POWER(2,B20)</f>
+        <v>32768</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <f>ROUND(B21*B13*B18,0)</f>
+        <v>8062</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <f>ROUND(B21*B14*B18,0)</f>
+        <v>8062</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B22">
-        <f>ROUND(B19*B12,0)</f>
+      <c r="B24">
+        <f>ROUND(B21*B12,0)</f>
         <v>28737</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <f>B13*B13</f>
+        <v>3.7836976644431289E-3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <f>2*B13*B14</f>
+        <v>7.5673953288862578E-3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <f>B14*B14</f>
+        <v>3.7836976644431289E-3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <f>2*B12</f>
+        <v>1.7539529259855136</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <f>-B12*B12</f>
+        <v>-0.76908771664328612</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37">
+        <f>2^B36</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38">
+        <f>ROUND(B29*B27*B37,0)</f>
+        <v>124</v>
+      </c>
+      <c r="D38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39">
+        <f>ROUND(B30*B27*B37,0)</f>
+        <v>248</v>
+      </c>
+      <c r="D39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40">
+        <f>ROUND(B31*B27*B37,0)</f>
+        <v>124</v>
+      </c>
+      <c r="D40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41">
+        <f>ROUND(B33*B37,0)</f>
+        <v>28737</v>
+      </c>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42">
+        <f>ROUND(B34*B37,0)</f>
+        <v>-12601</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -1202,7 +1413,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>

</xml_diff>